<commit_message>
Added the .98 periodic
</commit_message>
<xml_diff>
--- a/graphs/morphRunnings.xlsx
+++ b/graphs/morphRunnings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="4"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="p = .999" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="p = .95" sheetId="5" r:id="rId5"/>
     <sheet name="2min_comparison" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="171027" iterateDelta="1E-4"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36190,7 +36190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N118"/>
   <sheetViews>
-    <sheetView topLeftCell="G4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N94" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L6" sqref="L6:N24"/>
     </sheetView>
   </sheetViews>
@@ -54325,7 +54325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G13" workbookViewId="0">
       <selection activeCell="L6" sqref="L6:N25"/>
     </sheetView>
   </sheetViews>

</xml_diff>